<commit_message>
added flowering time to silvers
</commit_message>
<xml_diff>
--- a/Data/silvics_data.xlsx
+++ b/Data/silvics_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="-320" yWindow="1640" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="125">
   <si>
     <t>genus</t>
   </si>
@@ -346,13 +346,61 @@
   </si>
   <si>
     <t>thomasii</t>
+  </si>
+  <si>
+    <t>fruit_time</t>
+  </si>
+  <si>
+    <t>locality</t>
+  </si>
+  <si>
+    <t>flower_time</t>
+  </si>
+  <si>
+    <t>flower_locality</t>
+  </si>
+  <si>
+    <t>early_summer</t>
+  </si>
+  <si>
+    <t>southeast</t>
+  </si>
+  <si>
+    <t>oregon?</t>
+  </si>
+  <si>
+    <t>New england</t>
+  </si>
+  <si>
+    <t>range ave</t>
+  </si>
+  <si>
+    <t>late_spring/early_summer</t>
+  </si>
+  <si>
+    <t>north</t>
+  </si>
+  <si>
+    <t>as late as midwinter</t>
+  </si>
+  <si>
+    <t>fall/winter</t>
+  </si>
+  <si>
+    <t>winter</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>allegheny</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -374,6 +422,22 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -392,8 +456,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -401,7 +467,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -731,15 +799,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD49"/>
+    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -755,8 +826,20 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -772,8 +855,17 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -789,8 +881,17 @@
       <c r="E3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>11.5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -806,8 +907,20 @@
       <c r="E4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>9.5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4">
+        <v>4.5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -815,7 +928,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -823,8 +936,14 @@
       <c r="E5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>8.5</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -832,7 +951,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -840,8 +959,14 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>5.5</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -849,7 +974,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -857,8 +982,14 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -866,7 +997,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -874,8 +1005,14 @@
       <c r="E8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>10.5</v>
+      </c>
+      <c r="H8">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -891,8 +1028,14 @@
       <c r="E9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -900,7 +1043,7 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
@@ -908,8 +1051,14 @@
       <c r="E10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <v>9.5</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -917,7 +1066,7 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -925,8 +1074,14 @@
       <c r="E11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -934,7 +1089,7 @@
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
@@ -942,8 +1097,14 @@
       <c r="E12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <v>8.5</v>
+      </c>
+      <c r="H12">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -959,8 +1120,14 @@
       <c r="E13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -976,8 +1143,14 @@
       <c r="E14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H14">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -993,8 +1166,17 @@
       <c r="E15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>4.5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1010,8 +1192,14 @@
       <c r="E16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <v>11</v>
+      </c>
+      <c r="H16">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1027,8 +1215,14 @@
       <c r="E17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1044,8 +1238,14 @@
       <c r="E18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18">
+        <v>10.5</v>
+      </c>
+      <c r="H18">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1061,8 +1261,17 @@
       <c r="E19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <v>10.5</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1078,8 +1287,17 @@
       <c r="E20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="I20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1095,8 +1313,14 @@
       <c r="E21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" t="s">
+        <v>120</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1112,8 +1336,14 @@
       <c r="E22" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" t="s">
+        <v>121</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -1126,8 +1356,17 @@
       <c r="D23" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23">
+        <v>5</v>
+      </c>
+      <c r="I23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1143,8 +1382,14 @@
       <c r="E24" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="H24">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1160,8 +1405,14 @@
       <c r="E25" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1177,8 +1428,14 @@
       <c r="E26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26">
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -1194,8 +1451,14 @@
       <c r="E27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27">
+        <v>8.5</v>
+      </c>
+      <c r="H27">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1211,8 +1474,14 @@
       <c r="E28" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28">
+        <v>8.5</v>
+      </c>
+      <c r="H28">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1228,8 +1497,17 @@
       <c r="E29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29">
+        <v>9.5</v>
+      </c>
+      <c r="H29">
+        <v>4.5</v>
+      </c>
+      <c r="I29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -1245,8 +1523,14 @@
       <c r="E30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30">
+        <v>11</v>
+      </c>
+      <c r="H30">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -1262,8 +1546,17 @@
       <c r="E31" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31">
+        <v>10.5</v>
+      </c>
+      <c r="H31">
+        <v>6</v>
+      </c>
+      <c r="I31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -1276,8 +1569,14 @@
       <c r="D32" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32">
+        <v>10.5</v>
+      </c>
+      <c r="H32">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -1293,8 +1592,14 @@
       <c r="E33" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" t="s">
+        <v>122</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>68</v>
       </c>
@@ -1310,8 +1615,17 @@
       <c r="E34" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34">
+        <v>10</v>
+      </c>
+      <c r="H34">
+        <v>6</v>
+      </c>
+      <c r="I34" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -1327,8 +1641,14 @@
       <c r="E35" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35">
+        <v>9</v>
+      </c>
+      <c r="H35">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -1344,8 +1664,14 @@
       <c r="E36" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36">
+        <v>9.5</v>
+      </c>
+      <c r="H36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -1361,8 +1687,14 @@
       <c r="E37" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37">
+        <v>10.5</v>
+      </c>
+      <c r="H37">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -1378,8 +1710,14 @@
       <c r="E38" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38">
+        <v>11.5</v>
+      </c>
+      <c r="H38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -1395,8 +1733,20 @@
       <c r="E39" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39">
+        <v>9</v>
+      </c>
+      <c r="G39" t="s">
+        <v>123</v>
+      </c>
+      <c r="H39">
+        <v>6</v>
+      </c>
+      <c r="I39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -1412,8 +1762,17 @@
       <c r="E40" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40">
+        <v>6.5</v>
+      </c>
+      <c r="G40" t="s">
+        <v>119</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -1429,8 +1788,14 @@
       <c r="E41" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41">
+        <v>5.5</v>
+      </c>
+      <c r="H41">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -1446,8 +1811,14 @@
       <c r="E42" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42">
+        <v>5.5</v>
+      </c>
+      <c r="H42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -1463,8 +1834,20 @@
       <c r="E43" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43">
+        <v>5.5</v>
+      </c>
+      <c r="G43" t="s">
+        <v>123</v>
+      </c>
+      <c r="H43">
+        <v>4.5</v>
+      </c>
+      <c r="I43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>77</v>
       </c>
@@ -1480,8 +1863,14 @@
       <c r="E44" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44">
+        <v>5.5</v>
+      </c>
+      <c r="H44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>83</v>
       </c>
@@ -1489,7 +1878,7 @@
         <v>59</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D45" t="s">
         <v>16</v>
@@ -1497,8 +1886,14 @@
       <c r="E45" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45">
+        <v>7</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>83</v>
       </c>
@@ -1514,8 +1909,17 @@
       <c r="E46" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46">
+        <v>8.5</v>
+      </c>
+      <c r="G46" t="s">
+        <v>124</v>
+      </c>
+      <c r="H46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>85</v>
       </c>
@@ -1531,8 +1935,14 @@
       <c r="E47" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47">
+        <v>9.5</v>
+      </c>
+      <c r="H47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -1548,8 +1958,14 @@
       <c r="E48" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48">
+        <v>9.5</v>
+      </c>
+      <c r="H48">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>85</v>
       </c>
@@ -1565,8 +1981,17 @@
       <c r="E49" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49">
+        <v>9.5</v>
+      </c>
+      <c r="H49">
+        <v>6.5</v>
+      </c>
+      <c r="I49" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -1582,8 +2007,14 @@
       <c r="E50" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50">
+        <v>21</v>
+      </c>
+      <c r="H50">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>85</v>
       </c>
@@ -1599,8 +2030,14 @@
       <c r="E51" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51">
+        <v>21</v>
+      </c>
+      <c r="H51">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -1616,8 +2053,14 @@
       <c r="E52" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52">
+        <v>22</v>
+      </c>
+      <c r="H52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>85</v>
       </c>
@@ -1633,8 +2076,14 @@
       <c r="E53" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53">
+        <v>9.5</v>
+      </c>
+      <c r="H53">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>85</v>
       </c>
@@ -1650,8 +2099,14 @@
       <c r="E54" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54">
+        <v>21</v>
+      </c>
+      <c r="H54">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>85</v>
       </c>
@@ -1667,8 +2122,14 @@
       <c r="E55" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55">
+        <v>9.5</v>
+      </c>
+      <c r="H55">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -1684,8 +2145,14 @@
       <c r="E56" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56">
+        <v>9.5</v>
+      </c>
+      <c r="H56">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>85</v>
       </c>
@@ -1701,8 +2168,14 @@
       <c r="E57" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57">
+        <v>21</v>
+      </c>
+      <c r="H57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>85</v>
       </c>
@@ -1718,8 +2191,14 @@
       <c r="E58" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58">
+        <v>11.5</v>
+      </c>
+      <c r="H58">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>85</v>
       </c>
@@ -1735,8 +2214,14 @@
       <c r="E59" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59">
+        <v>21</v>
+      </c>
+      <c r="H59">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>85</v>
       </c>
@@ -1752,8 +2237,17 @@
       <c r="E60" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60">
+        <v>10</v>
+      </c>
+      <c r="H60">
+        <v>5</v>
+      </c>
+      <c r="I60" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>85</v>
       </c>
@@ -1769,8 +2263,14 @@
       <c r="E61" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61">
+        <v>9.5</v>
+      </c>
+      <c r="H61" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>99</v>
       </c>
@@ -1786,8 +2286,14 @@
       <c r="E62" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62">
+        <v>12.5</v>
+      </c>
+      <c r="H62">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>102</v>
       </c>
@@ -1803,8 +2309,17 @@
       <c r="E63" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63">
+        <v>6.5</v>
+      </c>
+      <c r="H63">
+        <v>4</v>
+      </c>
+      <c r="I63" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>103</v>
       </c>
@@ -1820,8 +2335,14 @@
       <c r="E64" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64">
+        <v>8.5</v>
+      </c>
+      <c r="H64">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>105</v>
       </c>
@@ -1837,8 +2358,14 @@
       <c r="E65" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65">
+        <v>9.5</v>
+      </c>
+      <c r="H65">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
         <v>106</v>
       </c>
@@ -1854,8 +2381,14 @@
       <c r="E66" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="F66">
+        <v>4</v>
+      </c>
+      <c r="H66">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
         <v>106</v>
       </c>
@@ -1871,8 +2404,20 @@
       <c r="E67" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67">
+        <v>4.5</v>
+      </c>
+      <c r="G67" t="s">
+        <v>123</v>
+      </c>
+      <c r="H67">
+        <v>3.5</v>
+      </c>
+      <c r="I67" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" t="s">
         <v>106</v>
       </c>
@@ -1888,8 +2433,14 @@
       <c r="E68" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="F68">
+        <v>5.5</v>
+      </c>
+      <c r="H68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" t="s">
         <v>106</v>
       </c>
@@ -1905,9 +2456,16 @@
       <c r="E69" t="s">
         <v>67</v>
       </c>
+      <c r="F69">
+        <v>5</v>
+      </c>
+      <c r="H69">
+        <v>3.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Ran model with slivics
also began VT data sheet but I think its too sparse to be worth it.
</commit_message>
<xml_diff>
--- a/Data/silvics_data.xlsx
+++ b/Data/silvics_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-320" yWindow="1640" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
+    <workbookView xWindow="620" yWindow="500" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -348,9 +348,6 @@
     <t>thomasii</t>
   </si>
   <si>
-    <t>fruit_time</t>
-  </si>
-  <si>
     <t>locality</t>
   </si>
   <si>
@@ -394,6 +391,9 @@
   </si>
   <si>
     <t>allegheny</t>
+  </si>
+  <si>
+    <t>av_fruit_time</t>
   </si>
 </sst>
 </file>
@@ -801,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -827,16 +827,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -856,10 +856,10 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" t="s">
         <v>113</v>
-      </c>
-      <c r="G2" t="s">
-        <v>114</v>
       </c>
       <c r="H2">
         <v>4</v>
@@ -885,7 +885,7 @@
         <v>11.5</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3">
         <v>4.5</v>
@@ -911,13 +911,13 @@
         <v>9.5</v>
       </c>
       <c r="G4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H4">
         <v>4.5</v>
       </c>
       <c r="I4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1144,7 +1144,7 @@
         <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H14">
         <v>4.5</v>
@@ -1173,7 +1173,7 @@
         <v>4.5</v>
       </c>
       <c r="I15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1268,7 +1268,7 @@
         <v>6</v>
       </c>
       <c r="I19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1294,7 +1294,7 @@
         <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1314,7 +1314,7 @@
         <v>30</v>
       </c>
       <c r="F21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H21">
         <v>4</v>
@@ -1337,7 +1337,7 @@
         <v>49</v>
       </c>
       <c r="F22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H22">
         <v>4</v>
@@ -1363,7 +1363,7 @@
         <v>5</v>
       </c>
       <c r="I23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1504,7 +1504,7 @@
         <v>4.5</v>
       </c>
       <c r="I29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1553,7 +1553,7 @@
         <v>6</v>
       </c>
       <c r="I31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1593,7 +1593,7 @@
         <v>67</v>
       </c>
       <c r="F33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H33">
         <v>5</v>
@@ -1622,7 +1622,7 @@
         <v>6</v>
       </c>
       <c r="I34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1737,13 +1737,13 @@
         <v>9</v>
       </c>
       <c r="G39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H39">
         <v>6</v>
       </c>
       <c r="I39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1766,7 +1766,7 @@
         <v>6.5</v>
       </c>
       <c r="G40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H40">
         <v>3</v>
@@ -1838,13 +1838,13 @@
         <v>5.5</v>
       </c>
       <c r="G43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H43">
         <v>4.5</v>
       </c>
       <c r="I43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1913,7 +1913,7 @@
         <v>8.5</v>
       </c>
       <c r="G46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H46">
         <v>5</v>
@@ -1988,7 +1988,7 @@
         <v>6.5</v>
       </c>
       <c r="I49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2244,7 +2244,7 @@
         <v>5</v>
       </c>
       <c r="I60" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2316,7 +2316,7 @@
         <v>4</v>
       </c>
       <c r="I63" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2408,13 +2408,13 @@
         <v>4.5</v>
       </c>
       <c r="G67" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H67">
         <v>3.5</v>
       </c>
       <c r="I67" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:9">

</xml_diff>

<commit_message>
filled in tolerance for silvers data sheet
also added well known classifiers to nas. ex if sassafras was NA for
pollination changed to insect
</commit_message>
<xml_diff>
--- a/Data/silvics_data.xlsx
+++ b/Data/silvics_data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="500" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="0" windowWidth="24260" windowHeight="26240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="134">
   <si>
     <t>genus</t>
   </si>
@@ -297,9 +297,6 @@
     <t>laurifolia</t>
   </si>
   <si>
-    <t>pro?</t>
-  </si>
-  <si>
     <t>lyrata</t>
   </si>
   <si>
@@ -378,9 +375,6 @@
     <t>north</t>
   </si>
   <si>
-    <t>as late as midwinter</t>
-  </si>
-  <si>
     <t>fall/winter</t>
   </si>
   <si>
@@ -394,6 +388,39 @@
   </si>
   <si>
     <t>av_fruit_time</t>
+  </si>
+  <si>
+    <t>cinerea</t>
+  </si>
+  <si>
+    <t>shade</t>
+  </si>
+  <si>
+    <t>tolerant</t>
+  </si>
+  <si>
+    <t>very_tolerant</t>
+  </si>
+  <si>
+    <t>Ailthanthus</t>
+  </si>
+  <si>
+    <t>altissima</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>intolerant</t>
+  </si>
+  <si>
+    <t>medium_tolerant</t>
+  </si>
+  <si>
+    <t>very_intolerant</t>
+  </si>
+  <si>
+    <t>medium</t>
   </si>
 </sst>
 </file>
@@ -799,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -810,7 +837,7 @@
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -827,19 +854,25 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="K1" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -856,16 +889,16 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" t="s">
         <v>112</v>
-      </c>
-      <c r="G2" t="s">
-        <v>113</v>
       </c>
       <c r="H2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -885,13 +918,16 @@
         <v>11.5</v>
       </c>
       <c r="G3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H3">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="K3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -911,16 +947,22 @@
         <v>9.5</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4">
         <v>4.5</v>
       </c>
       <c r="I4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>115</v>
+      </c>
+      <c r="J4" t="s">
+        <v>126</v>
+      </c>
+      <c r="K4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -942,8 +984,14 @@
       <c r="H5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -965,8 +1013,14 @@
       <c r="H6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" t="s">
+        <v>125</v>
+      </c>
+      <c r="K6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -988,8 +1042,14 @@
       <c r="H7">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" t="s">
+        <v>125</v>
+      </c>
+      <c r="K7">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1011,8 +1071,14 @@
       <c r="H8">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" t="s">
+        <v>126</v>
+      </c>
+      <c r="K8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1034,8 +1100,14 @@
       <c r="H9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" t="s">
+        <v>125</v>
+      </c>
+      <c r="K9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1057,8 +1129,14 @@
       <c r="H10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" t="s">
+        <v>125</v>
+      </c>
+      <c r="K10">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1080,36 +1158,45 @@
       <c r="H11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" t="s">
+        <v>125</v>
+      </c>
+      <c r="K11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12">
-        <v>8.5</v>
+        <v>27</v>
       </c>
       <c r="H12">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" t="s">
+        <v>130</v>
+      </c>
+      <c r="K12">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
@@ -1121,18 +1208,24 @@
         <v>18</v>
       </c>
       <c r="F13">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="H13">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>5.5</v>
+      </c>
+      <c r="J13" t="s">
+        <v>131</v>
+      </c>
+      <c r="K13">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -1143,19 +1236,25 @@
       <c r="E14" t="s">
         <v>18</v>
       </c>
-      <c r="F14" t="s">
-        <v>117</v>
+      <c r="F14">
+        <v>10</v>
       </c>
       <c r="H14">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" t="s">
+        <v>130</v>
+      </c>
+      <c r="K14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
@@ -1167,21 +1266,24 @@
         <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="H15">
         <v>4.5</v>
       </c>
-      <c r="I15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" t="s">
+        <v>130</v>
+      </c>
+      <c r="K15">
+        <v>24.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
@@ -1192,71 +1294,89 @@
       <c r="E16" t="s">
         <v>18</v>
       </c>
-      <c r="F16">
-        <v>11</v>
+      <c r="F16" t="s">
+        <v>7</v>
       </c>
       <c r="H16">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="I16" t="s">
+        <v>117</v>
+      </c>
+      <c r="J16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
         <v>18</v>
       </c>
       <c r="F17">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>4.5</v>
+      </c>
+      <c r="J17" t="s">
+        <v>131</v>
+      </c>
+      <c r="K17">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
         <v>18</v>
       </c>
       <c r="F18">
-        <v>10.5</v>
+        <v>10</v>
       </c>
       <c r="H18">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>5</v>
+      </c>
+      <c r="J18" t="s">
+        <v>126</v>
+      </c>
+      <c r="K18">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
         <v>18</v>
@@ -1265,90 +1385,105 @@
         <v>10.5</v>
       </c>
       <c r="H19">
-        <v>6</v>
-      </c>
-      <c r="I19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>4.5</v>
+      </c>
+      <c r="J19" t="s">
+        <v>130</v>
+      </c>
+      <c r="K19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="F20">
+        <v>10.5</v>
       </c>
       <c r="H20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I20" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>117</v>
+      </c>
+      <c r="J20" t="s">
+        <v>131</v>
+      </c>
+      <c r="K20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E21" t="s">
         <v>30</v>
       </c>
-      <c r="F21" t="s">
-        <v>119</v>
+      <c r="F21">
+        <v>9.5</v>
       </c>
       <c r="H21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>5</v>
+      </c>
+      <c r="I21" t="s">
+        <v>117</v>
+      </c>
+      <c r="J21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" t="s">
-        <v>120</v>
+        <v>30</v>
+      </c>
+      <c r="F22">
+        <v>9.5</v>
       </c>
       <c r="H22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
@@ -1356,54 +1491,63 @@
       <c r="D23" t="s">
         <v>12</v>
       </c>
+      <c r="E23" t="s">
+        <v>49</v>
+      </c>
       <c r="F23" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="J23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>9.5</v>
+      </c>
+      <c r="H24">
         <v>5</v>
       </c>
-      <c r="I23" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" t="s">
+      <c r="I24" t="s">
+        <v>117</v>
+      </c>
+      <c r="J24" t="s">
+        <v>126</v>
+      </c>
+      <c r="K24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
         <v>52</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24">
-        <v>10</v>
-      </c>
-      <c r="H24">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D25" t="s">
         <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F25">
         <v>10</v>
@@ -1411,22 +1555,28 @@
       <c r="H25">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" t="s">
+        <v>126</v>
+      </c>
+      <c r="K25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F26">
         <v>10</v>
@@ -1434,373 +1584,463 @@
       <c r="H26">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" t="s">
+        <v>126</v>
+      </c>
+      <c r="K26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E27" t="s">
         <v>27</v>
       </c>
       <c r="F27">
-        <v>8.5</v>
+        <v>10</v>
       </c>
       <c r="H27">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" t="s">
+        <v>130</v>
+      </c>
+      <c r="K27">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="F28">
         <v>8.5</v>
       </c>
       <c r="H28">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>4.5</v>
+      </c>
+      <c r="J28" t="s">
+        <v>131</v>
+      </c>
+      <c r="K28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
       </c>
       <c r="E29" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F29">
-        <v>9.5</v>
+        <v>8.5</v>
       </c>
       <c r="H29">
-        <v>4.5</v>
-      </c>
-      <c r="I29" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>5.5</v>
+      </c>
+      <c r="J29" t="s">
+        <v>130</v>
+      </c>
+      <c r="K29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E30" t="s">
         <v>27</v>
       </c>
       <c r="F30">
-        <v>11</v>
+        <v>9.5</v>
       </c>
       <c r="H30">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="I30" t="s">
+        <v>117</v>
+      </c>
+      <c r="J30" t="s">
+        <v>125</v>
+      </c>
+      <c r="K30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31">
+        <v>11</v>
+      </c>
+      <c r="H31">
+        <v>4.5</v>
+      </c>
+      <c r="J31" t="s">
+        <v>131</v>
+      </c>
+      <c r="K31">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" t="s">
         <v>61</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>62</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31">
-        <v>10.5</v>
-      </c>
-      <c r="H31">
-        <v>6</v>
-      </c>
-      <c r="I31" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" t="s">
-        <v>64</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F32">
         <v>10.5</v>
       </c>
       <c r="H32">
+        <v>6</v>
+      </c>
+      <c r="I32" t="s">
+        <v>117</v>
+      </c>
+      <c r="J32" t="s">
+        <v>130</v>
+      </c>
+      <c r="K32">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33">
+        <v>10.5</v>
+      </c>
+      <c r="H33">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" t="s">
+      <c r="J33" t="s">
+        <v>125</v>
+      </c>
+      <c r="K33">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
         <v>65</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>66</v>
       </c>
-      <c r="C33" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" t="s">
-        <v>121</v>
-      </c>
-      <c r="H33">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D34" t="s">
         <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34">
-        <v>10</v>
+        <v>67</v>
+      </c>
+      <c r="F34" t="s">
+        <v>119</v>
       </c>
       <c r="H34">
-        <v>6</v>
-      </c>
-      <c r="I34" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>5</v>
+      </c>
+      <c r="J34" t="s">
+        <v>125</v>
+      </c>
+      <c r="K34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>123</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
       </c>
       <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35">
+        <v>9.5</v>
+      </c>
+      <c r="H35">
+        <v>5</v>
+      </c>
+      <c r="J35" t="s">
+        <v>130</v>
+      </c>
+      <c r="K35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36">
+        <v>10</v>
+      </c>
+      <c r="H36">
+        <v>6</v>
+      </c>
+      <c r="I36" t="s">
+        <v>117</v>
+      </c>
+      <c r="J36" t="s">
+        <v>130</v>
+      </c>
+      <c r="K36">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
         <v>24</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E37" t="s">
         <v>67</v>
       </c>
-      <c r="F35">
+      <c r="F37">
         <v>9</v>
       </c>
-      <c r="H35">
+      <c r="H37">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" t="s">
+      <c r="J37" t="s">
+        <v>131</v>
+      </c>
+      <c r="K37">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" t="s">
         <v>71</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>72</v>
       </c>
-      <c r="C36" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" t="s">
-        <v>27</v>
-      </c>
-      <c r="F36">
-        <v>9.5</v>
-      </c>
-      <c r="H36">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37">
-        <v>10.5</v>
-      </c>
-      <c r="H37">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" t="s">
-        <v>75</v>
-      </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D38" t="s">
         <v>22</v>
       </c>
       <c r="E38" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38">
+        <v>9.5</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+      <c r="J38" t="s">
+        <v>130</v>
+      </c>
+      <c r="K38">
         <v>9</v>
       </c>
-      <c r="F38">
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39">
+        <v>10.5</v>
+      </c>
+      <c r="H39">
+        <v>3.5</v>
+      </c>
+      <c r="J39" t="s">
+        <v>130</v>
+      </c>
+      <c r="K39">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40">
         <v>11.5</v>
       </c>
-      <c r="H38">
+      <c r="H40">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" t="s">
+      <c r="J40" t="s">
+        <v>130</v>
+      </c>
+      <c r="K40">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" t="s">
         <v>76</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>53</v>
       </c>
-      <c r="C39" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
         <v>16</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E41" t="s">
         <v>18</v>
       </c>
-      <c r="F39">
+      <c r="F41">
         <v>9</v>
       </c>
-      <c r="G39" t="s">
-        <v>122</v>
-      </c>
-      <c r="H39">
+      <c r="G41" t="s">
+        <v>120</v>
+      </c>
+      <c r="H41">
         <v>6</v>
       </c>
-      <c r="I39" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="I41" t="s">
+        <v>117</v>
+      </c>
+      <c r="J41" t="s">
+        <v>125</v>
+      </c>
+      <c r="K41">
         <v>12</v>
       </c>
-      <c r="E40" t="s">
-        <v>27</v>
-      </c>
-      <c r="F40">
-        <v>6.5</v>
-      </c>
-      <c r="G40" t="s">
-        <v>118</v>
-      </c>
-      <c r="H40">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" t="s">
-        <v>27</v>
-      </c>
-      <c r="F41">
-        <v>5.5</v>
-      </c>
-      <c r="H41">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
         <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
         <v>15</v>
@@ -1812,18 +2052,27 @@
         <v>27</v>
       </c>
       <c r="F42">
-        <v>5.5</v>
+        <v>6.5</v>
+      </c>
+      <c r="G42" t="s">
+        <v>117</v>
       </c>
       <c r="H42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v>3</v>
+      </c>
+      <c r="J42" t="s">
+        <v>132</v>
+      </c>
+      <c r="K42">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
         <v>77</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
         <v>15</v>
@@ -1837,22 +2086,22 @@
       <c r="F43">
         <v>5.5</v>
       </c>
-      <c r="G43" t="s">
-        <v>122</v>
-      </c>
       <c r="H43">
         <v>4.5</v>
       </c>
-      <c r="I43" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43" t="s">
+        <v>132</v>
+      </c>
+      <c r="K43">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>77</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s">
         <v>15</v>
@@ -1869,114 +2118,150 @@
       <c r="H44">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44" t="s">
+        <v>132</v>
+      </c>
+      <c r="K44">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45">
+        <v>5.5</v>
+      </c>
+      <c r="G45" t="s">
+        <v>120</v>
+      </c>
+      <c r="H45">
+        <v>4.5</v>
+      </c>
+      <c r="I45" t="s">
+        <v>120</v>
+      </c>
+      <c r="J45" t="s">
+        <v>132</v>
+      </c>
+      <c r="K45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46">
+        <v>5.5</v>
+      </c>
+      <c r="H46">
+        <v>4</v>
+      </c>
+      <c r="J46" t="s">
+        <v>130</v>
+      </c>
+      <c r="K46">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" t="s">
         <v>83</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" t="s">
         <v>59</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>11</v>
-      </c>
-      <c r="D45" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" t="s">
-        <v>67</v>
-      </c>
-      <c r="F45">
-        <v>7</v>
-      </c>
-      <c r="H45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" t="s">
-        <v>83</v>
-      </c>
-      <c r="B46" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" t="s">
-        <v>16</v>
-      </c>
-      <c r="E46" t="s">
-        <v>67</v>
-      </c>
-      <c r="F46">
-        <v>8.5</v>
-      </c>
-      <c r="G46" t="s">
-        <v>123</v>
-      </c>
-      <c r="H46">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" t="s">
-        <v>85</v>
-      </c>
-      <c r="B47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C47" t="s">
-        <v>15</v>
       </c>
       <c r="D47" t="s">
         <v>16</v>
       </c>
       <c r="E47" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="F47">
-        <v>9.5</v>
+        <v>7</v>
       </c>
       <c r="H47">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>5</v>
+      </c>
+      <c r="J47" t="s">
+        <v>132</v>
+      </c>
+      <c r="K47">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C48" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D48" t="s">
         <v>16</v>
       </c>
       <c r="E48" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="F48">
-        <v>9.5</v>
+        <v>8.5</v>
+      </c>
+      <c r="G48" t="s">
+        <v>121</v>
       </c>
       <c r="H48">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>5</v>
+      </c>
+      <c r="J48" t="s">
+        <v>130</v>
+      </c>
+      <c r="K48">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
         <v>85</v>
       </c>
       <c r="B49" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C49" t="s">
         <v>15</v>
       </c>
       <c r="D49" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E49" t="s">
         <v>18</v>
@@ -1985,133 +2270,166 @@
         <v>9.5</v>
       </c>
       <c r="H49">
-        <v>6.5</v>
-      </c>
-      <c r="I49" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+        <v>4</v>
+      </c>
+      <c r="J49" t="s">
+        <v>131</v>
+      </c>
+      <c r="K49">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>85</v>
       </c>
       <c r="B50" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="C50" t="s">
         <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E50" t="s">
         <v>18</v>
       </c>
       <c r="F50">
-        <v>21</v>
+        <v>9.5</v>
       </c>
       <c r="H50">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+        <v>5.5</v>
+      </c>
+      <c r="J50" t="s">
+        <v>131</v>
+      </c>
+      <c r="K50">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>85</v>
       </c>
       <c r="B51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E51" t="s">
         <v>18</v>
       </c>
       <c r="F51">
-        <v>21</v>
+        <v>9.5</v>
       </c>
       <c r="H51">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+        <v>6.5</v>
+      </c>
+      <c r="I51" t="s">
+        <v>117</v>
+      </c>
+      <c r="J51" t="s">
+        <v>131</v>
+      </c>
+      <c r="K51">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>85</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E52" t="s">
         <v>18</v>
       </c>
       <c r="F52">
-        <v>22</v>
-      </c>
-      <c r="H52" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+        <v>21</v>
+      </c>
+      <c r="H52">
+        <v>4.5</v>
+      </c>
+      <c r="J52" t="s">
+        <v>131</v>
+      </c>
+      <c r="K52">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>85</v>
       </c>
       <c r="B53" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C53" t="s">
         <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E53" t="s">
         <v>18</v>
       </c>
       <c r="F53">
-        <v>9.5</v>
+        <v>21</v>
       </c>
       <c r="H53">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53" t="s">
+        <v>133</v>
+      </c>
+      <c r="K53">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>85</v>
       </c>
       <c r="B54" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C54" t="s">
         <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="E54" t="s">
         <v>18</v>
       </c>
       <c r="F54">
-        <v>21</v>
-      </c>
-      <c r="H54">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v>22</v>
+      </c>
+      <c r="H54" t="s">
+        <v>7</v>
+      </c>
+      <c r="J54" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" t="s">
         <v>85</v>
       </c>
       <c r="B55" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C55" t="s">
         <v>15</v>
@@ -2128,59 +2446,77 @@
       <c r="H55">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="J55" t="s">
+        <v>130</v>
+      </c>
+      <c r="K55">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" t="s">
         <v>85</v>
       </c>
       <c r="B56" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C56" t="s">
         <v>15</v>
       </c>
       <c r="D56" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E56" t="s">
         <v>18</v>
       </c>
       <c r="F56">
-        <v>9.5</v>
+        <v>21</v>
       </c>
       <c r="H56">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+        <v>2.5</v>
+      </c>
+      <c r="J56" t="s">
+        <v>125</v>
+      </c>
+      <c r="K56">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
         <v>85</v>
       </c>
       <c r="B57" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
       </c>
       <c r="D57" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E57" t="s">
         <v>18</v>
       </c>
       <c r="F57">
-        <v>21</v>
-      </c>
-      <c r="H57" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>9.5</v>
+      </c>
+      <c r="H57">
+        <v>4.5</v>
+      </c>
+      <c r="J57" t="s">
+        <v>131</v>
+      </c>
+      <c r="K57">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" t="s">
         <v>85</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C58" t="s">
         <v>15</v>
@@ -2192,24 +2528,30 @@
         <v>18</v>
       </c>
       <c r="F58">
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="H58">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+        <v>4.5</v>
+      </c>
+      <c r="J58" t="s">
+        <v>130</v>
+      </c>
+      <c r="K58">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" t="s">
         <v>85</v>
       </c>
       <c r="B59" t="s">
-        <v>96</v>
+        <v>36</v>
       </c>
       <c r="C59" t="s">
         <v>15</v>
       </c>
       <c r="D59" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E59" t="s">
         <v>18</v>
@@ -2217,16 +2559,22 @@
       <c r="F59">
         <v>21</v>
       </c>
-      <c r="H59">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="H59" t="s">
+        <v>7</v>
+      </c>
+      <c r="J59" t="s">
+        <v>130</v>
+      </c>
+      <c r="K59">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" t="s">
         <v>85</v>
       </c>
       <c r="B60" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C60" t="s">
         <v>15</v>
@@ -2238,191 +2586,233 @@
         <v>18</v>
       </c>
       <c r="F60">
-        <v>10</v>
+        <v>11.5</v>
       </c>
       <c r="H60">
-        <v>5</v>
-      </c>
-      <c r="I60" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+        <v>3.5</v>
+      </c>
+      <c r="J60" t="s">
+        <v>130</v>
+      </c>
+      <c r="K60">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" t="s">
         <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C61" t="s">
         <v>15</v>
       </c>
       <c r="D61" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E61" t="s">
         <v>18</v>
       </c>
       <c r="F61">
+        <v>21</v>
+      </c>
+      <c r="H61">
+        <v>3.5</v>
+      </c>
+      <c r="J61" t="s">
+        <v>130</v>
+      </c>
+      <c r="K61">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" t="s">
+        <v>18</v>
+      </c>
+      <c r="F62">
+        <v>10</v>
+      </c>
+      <c r="H62">
+        <v>5</v>
+      </c>
+      <c r="I62" t="s">
+        <v>117</v>
+      </c>
+      <c r="J62" t="s">
+        <v>130</v>
+      </c>
+      <c r="K62">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" t="s">
+        <v>85</v>
+      </c>
+      <c r="B63" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63" t="s">
+        <v>18</v>
+      </c>
+      <c r="F63">
         <v>9.5</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H63" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" t="s">
+      <c r="J63" t="s">
+        <v>131</v>
+      </c>
+      <c r="K63">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" t="s">
+        <v>98</v>
+      </c>
+      <c r="B64" t="s">
         <v>99</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C64" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64" t="s">
         <v>100</v>
       </c>
-      <c r="C62" t="s">
+      <c r="F64">
+        <v>12.5</v>
+      </c>
+      <c r="H64">
+        <v>5.5</v>
+      </c>
+      <c r="J64" t="s">
+        <v>132</v>
+      </c>
+      <c r="K64">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" t="s">
+        <v>101</v>
+      </c>
+      <c r="B65" t="s">
+        <v>36</v>
+      </c>
+      <c r="C65" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" t="s">
+        <v>27</v>
+      </c>
+      <c r="F65">
+        <v>6.5</v>
+      </c>
+      <c r="H65">
+        <v>4</v>
+      </c>
+      <c r="I65" t="s">
+        <v>120</v>
+      </c>
+      <c r="J65" t="s">
+        <v>132</v>
+      </c>
+      <c r="K65">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" t="s">
+        <v>102</v>
+      </c>
+      <c r="B66" t="s">
+        <v>103</v>
+      </c>
+      <c r="C66" t="s">
         <v>11</v>
       </c>
-      <c r="D62" t="s">
-        <v>22</v>
-      </c>
-      <c r="E62" t="s">
-        <v>101</v>
-      </c>
-      <c r="F62">
-        <v>12.5</v>
-      </c>
-      <c r="H62">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" t="s">
-        <v>102</v>
-      </c>
-      <c r="B63" t="s">
-        <v>36</v>
-      </c>
-      <c r="C63" t="s">
-        <v>17</v>
-      </c>
-      <c r="D63" t="s">
-        <v>8</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" t="s">
         <v>27</v>
       </c>
-      <c r="F63">
-        <v>6.5</v>
-      </c>
-      <c r="H63">
-        <v>4</v>
-      </c>
-      <c r="I63" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" t="s">
-        <v>103</v>
-      </c>
-      <c r="B64" t="s">
-        <v>104</v>
-      </c>
-      <c r="C64" t="s">
-        <v>7</v>
-      </c>
-      <c r="D64" t="s">
-        <v>16</v>
-      </c>
-      <c r="E64" t="s">
-        <v>27</v>
-      </c>
-      <c r="F64">
+      <c r="F66">
         <v>8.5</v>
-      </c>
-      <c r="H64">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
-      <c r="A65" t="s">
-        <v>105</v>
-      </c>
-      <c r="B65" t="s">
-        <v>57</v>
-      </c>
-      <c r="C65" t="s">
-        <v>11</v>
-      </c>
-      <c r="D65" t="s">
-        <v>22</v>
-      </c>
-      <c r="E65" t="s">
-        <v>67</v>
-      </c>
-      <c r="F65">
-        <v>9.5</v>
-      </c>
-      <c r="H65">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="A66" t="s">
-        <v>106</v>
-      </c>
-      <c r="B66" t="s">
-        <v>107</v>
-      </c>
-      <c r="C66" t="s">
-        <v>15</v>
-      </c>
-      <c r="D66" t="s">
-        <v>12</v>
-      </c>
-      <c r="E66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F66">
-        <v>4</v>
       </c>
       <c r="H66">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="J66" t="s">
+        <v>130</v>
+      </c>
+      <c r="K66">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B67" t="s">
         <v>57</v>
       </c>
       <c r="C67" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D67" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E67" t="s">
         <v>67</v>
       </c>
       <c r="F67">
-        <v>4.5</v>
-      </c>
-      <c r="G67" t="s">
-        <v>122</v>
+        <v>9.5</v>
       </c>
       <c r="H67">
-        <v>3.5</v>
-      </c>
-      <c r="I67" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <v>6</v>
+      </c>
+      <c r="J67" t="s">
+        <v>125</v>
+      </c>
+      <c r="K67">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68" t="s">
+        <v>105</v>
+      </c>
+      <c r="B68" t="s">
         <v>106</v>
-      </c>
-      <c r="B68" t="s">
-        <v>108</v>
       </c>
       <c r="C68" t="s">
         <v>15</v>
@@ -2434,18 +2824,24 @@
         <v>67</v>
       </c>
       <c r="F68">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="H68">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <v>3.5</v>
+      </c>
+      <c r="J68" t="s">
+        <v>125</v>
+      </c>
+      <c r="K68">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B69" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C69" t="s">
         <v>15</v>
@@ -2457,10 +2853,80 @@
         <v>67</v>
       </c>
       <c r="F69">
-        <v>5</v>
+        <v>4.5</v>
+      </c>
+      <c r="G69" t="s">
+        <v>120</v>
       </c>
       <c r="H69">
         <v>3.5</v>
+      </c>
+      <c r="I69" t="s">
+        <v>120</v>
+      </c>
+      <c r="J69" t="s">
+        <v>131</v>
+      </c>
+      <c r="K69">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" t="s">
+        <v>105</v>
+      </c>
+      <c r="B70" t="s">
+        <v>107</v>
+      </c>
+      <c r="C70" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" t="s">
+        <v>12</v>
+      </c>
+      <c r="E70" t="s">
+        <v>67</v>
+      </c>
+      <c r="F70">
+        <v>5.5</v>
+      </c>
+      <c r="H70">
+        <v>4</v>
+      </c>
+      <c r="J70" t="s">
+        <v>131</v>
+      </c>
+      <c r="K70">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" t="s">
+        <v>105</v>
+      </c>
+      <c r="B71" t="s">
+        <v>32</v>
+      </c>
+      <c r="C71" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" t="s">
+        <v>12</v>
+      </c>
+      <c r="E71" t="s">
+        <v>67</v>
+      </c>
+      <c r="F71">
+        <v>5</v>
+      </c>
+      <c r="H71">
+        <v>3.5</v>
+      </c>
+      <c r="J71" t="s">
+        <v>125</v>
+      </c>
+      <c r="K71">
+        <v>21.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>